<commit_message>
Finished styling 'Hero'; finished 'Members' section
</commit_message>
<xml_diff>
--- a/sizing.xlsx
+++ b/sizing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{104F4C4C-CE40-44ED-A901-1405CCA0D980}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7E7F76E7-1E39-4964-8D89-BCB6236509B9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,16 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Font Size (px)</t>
-  </si>
-  <si>
-    <t>Font Size (em)</t>
-  </si>
-  <si>
-    <t>El Class</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>.navbar .navbar-menu .navbar-item</t>
   </si>
@@ -38,13 +29,37 @@
   </si>
   <si>
     <t>px</t>
+  </si>
+  <si>
+    <t>Size (px)</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>font-size</t>
+  </si>
+  <si>
+    <t>.hero .title</t>
+  </si>
+  <si>
+    <t>.hero .content</t>
+  </si>
+  <si>
+    <t>line-height</t>
+  </si>
+  <si>
+    <t>Size (rem)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +88,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -107,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -119,6 +140,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,51 +421,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="3">
         <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5">
+        <v>15.96</v>
+      </c>
+      <c r="D4" s="5">
+        <f>C4/B1</f>
+        <v>0.99750000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5">
+        <v>72</v>
+      </c>
+      <c r="D5" s="5">
+        <f>C5/B1</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5">
+        <f>C6/B1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>15.96</v>
-      </c>
-      <c r="C4">
-        <f>B4/B1</f>
-        <v>0.99750000000000005</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5">
+        <v>47</v>
+      </c>
+      <c r="D7" s="5">
+        <f>C7/B1</f>
+        <v>2.9375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished 'About Us' section; included web fonts instead of system installed fonts
</commit_message>
<xml_diff>
--- a/sizing.xlsx
+++ b/sizing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A949E4DA-1E5B-423C-885D-59CFD5F61F2F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E8099F3-53BC-4422-958A-CB5D7918DB47}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>.navbar .navbar-menu .navbar-item</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>.package .footer-select</t>
+  </si>
+  <si>
+    <t>.about-us .content-left .title</t>
+  </si>
+  <si>
+    <t>.about-us .content-left .content-text</t>
   </si>
 </sst>
 </file>
@@ -433,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,6 +605,36 @@
         <v>0.99812500000000004</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5">
+        <v>35.11</v>
+      </c>
+      <c r="D12" s="5">
+        <f>C12/B1</f>
+        <v>2.194375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5">
+        <v>18.059999999999999</v>
+      </c>
+      <c r="D13" s="5">
+        <f>C13/B1</f>
+        <v>1.1287499999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>